<commit_message>
atualizar programação e prontidão
</commit_message>
<xml_diff>
--- a/programacao/15 -  Prontidão Médio Prazo.xlsx
+++ b/programacao/15 -  Prontidão Médio Prazo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://montisolbr-my.sharepoint.com/personal/suleima_caldas_montisol_com_br/Documents/1.CONTRATOS HYDRO/CT_4600011662_Utilidades/02.PLANEJAMENTO/01 - Base de dados BI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="996" documentId="13_ncr:1_{CF35CD03-2AB7-44C8-89C3-A37B38273E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF2C5C10-230D-4043-9E01-A567C09AA081}"/>
+  <xr:revisionPtr revIDLastSave="1011" documentId="13_ncr:1_{CF35CD03-2AB7-44C8-89C3-A37B38273E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D452ADEA-71BB-4C03-B1A9-787F39402709}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{32A6E8DD-ACB4-40F1-8D5E-8E9CE1A3868D}"/>
   </bookViews>
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6268" uniqueCount="2638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6283" uniqueCount="2638">
   <si>
     <t>Status</t>
   </si>
@@ -7954,9 +7954,6 @@
     <t>Pendente valvula, parafusos e flanges - Solicitar nota de materiais para saída</t>
   </si>
   <si>
-    <t xml:space="preserve">Pendente flanges, parafusos e valvula - Solicitar nota de materiais para sida </t>
-  </si>
-  <si>
     <t>Pendente materiais para fabricação</t>
   </si>
   <si>
@@ -8078,6 +8075,9 @@
   </si>
   <si>
     <t>0,19 dias</t>
+  </si>
+  <si>
+    <t>Pendente flanges, parafusos e valvula - Solicitar nota de materiais para saída</t>
   </si>
 </sst>
 </file>
@@ -10887,7 +10887,7 @@
         <v>1283</v>
       </c>
       <c r="D29" s="46" t="s">
-        <v>2615</v>
+        <v>2614</v>
       </c>
       <c r="E29" s="46" t="s">
         <v>135</v>
@@ -10953,7 +10953,7 @@
         <v>1286</v>
       </c>
       <c r="D32" s="46" t="s">
-        <v>2616</v>
+        <v>2615</v>
       </c>
       <c r="E32" s="46" t="s">
         <v>143</v>
@@ -10975,7 +10975,7 @@
         <v>1294</v>
       </c>
       <c r="D33" s="46" t="s">
-        <v>2617</v>
+        <v>2616</v>
       </c>
       <c r="E33" s="46" t="s">
         <v>143</v>
@@ -11085,7 +11085,7 @@
         <v>1295</v>
       </c>
       <c r="D38" s="46" t="s">
-        <v>2617</v>
+        <v>2616</v>
       </c>
       <c r="E38" s="46" t="s">
         <v>143</v>
@@ -11195,7 +11195,7 @@
         <v>1296</v>
       </c>
       <c r="D43" s="46" t="s">
-        <v>2617</v>
+        <v>2616</v>
       </c>
       <c r="E43" s="46" t="s">
         <v>143</v>
@@ -11635,7 +11635,7 @@
         <v>1297</v>
       </c>
       <c r="D63" s="46" t="s">
-        <v>2618</v>
+        <v>2617</v>
       </c>
       <c r="E63" s="46" t="s">
         <v>143</v>
@@ -11745,7 +11745,7 @@
         <v>1298</v>
       </c>
       <c r="D68" s="46" t="s">
-        <v>2619</v>
+        <v>2618</v>
       </c>
       <c r="E68" s="46" t="s">
         <v>143</v>
@@ -14671,7 +14671,7 @@
         <v>1283</v>
       </c>
       <c r="D201" s="46" t="s">
-        <v>2620</v>
+        <v>2619</v>
       </c>
       <c r="E201" s="46" t="s">
         <v>1827</v>
@@ -15432,7 +15432,7 @@
         <v>1314</v>
       </c>
       <c r="D237" s="46" t="s">
-        <v>2621</v>
+        <v>2620</v>
       </c>
       <c r="E237" s="46" t="s">
         <v>1964</v>
@@ -15453,7 +15453,7 @@
         <v>1424</v>
       </c>
       <c r="D238" s="46" t="s">
-        <v>2621</v>
+        <v>2620</v>
       </c>
       <c r="E238" s="46" t="s">
         <v>1964</v>
@@ -15726,7 +15726,7 @@
         <v>1434</v>
       </c>
       <c r="D251" s="46" t="s">
-        <v>2622</v>
+        <v>2621</v>
       </c>
       <c r="E251" s="46" t="s">
         <v>1850</v>
@@ -16230,7 +16230,7 @@
         <v>1446</v>
       </c>
       <c r="D275" s="46" t="s">
-        <v>2623</v>
+        <v>2622</v>
       </c>
       <c r="E275" s="46" t="s">
         <v>1853</v>
@@ -16251,7 +16251,7 @@
         <v>1447</v>
       </c>
       <c r="D276" s="46" t="s">
-        <v>2624</v>
+        <v>2623</v>
       </c>
       <c r="E276" s="46" t="s">
         <v>1853</v>
@@ -16734,7 +16734,7 @@
         <v>1467</v>
       </c>
       <c r="D299" s="46" t="s">
-        <v>2625</v>
+        <v>2624</v>
       </c>
       <c r="E299" s="46" t="s">
         <v>1937</v>
@@ -16755,7 +16755,7 @@
         <v>1468</v>
       </c>
       <c r="D300" s="46" t="s">
-        <v>2626</v>
+        <v>2625</v>
       </c>
       <c r="E300" s="46" t="s">
         <v>1937</v>
@@ -17196,7 +17196,7 @@
         <v>1328</v>
       </c>
       <c r="D321" s="46" t="s">
-        <v>2627</v>
+        <v>2626</v>
       </c>
       <c r="E321" s="46" t="s">
         <v>1998</v>
@@ -17217,7 +17217,7 @@
         <v>1489</v>
       </c>
       <c r="D322" s="46" t="s">
-        <v>2628</v>
+        <v>2627</v>
       </c>
       <c r="E322" s="46" t="s">
         <v>1998</v>
@@ -17364,7 +17364,7 @@
         <v>1495</v>
       </c>
       <c r="D329" s="46" t="s">
-        <v>2629</v>
+        <v>2628</v>
       </c>
       <c r="E329" s="46" t="s">
         <v>2284</v>
@@ -17595,7 +17595,7 @@
         <v>1499</v>
       </c>
       <c r="D340" s="46" t="s">
-        <v>2630</v>
+        <v>2629</v>
       </c>
       <c r="E340" s="46" t="s">
         <v>2291</v>
@@ -17805,7 +17805,7 @@
         <v>1503</v>
       </c>
       <c r="D350" s="46" t="s">
-        <v>2631</v>
+        <v>2630</v>
       </c>
       <c r="E350" s="46" t="s">
         <v>2011</v>
@@ -17952,7 +17952,7 @@
         <v>1308</v>
       </c>
       <c r="D357" s="46" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
       <c r="E357" s="46" t="s">
         <v>2037</v>
@@ -18309,7 +18309,7 @@
         <v>1313</v>
       </c>
       <c r="D374" s="46" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
       <c r="E374" s="46" t="s">
         <v>1978</v>
@@ -18645,7 +18645,7 @@
         <v>1311</v>
       </c>
       <c r="D390" s="46" t="s">
-        <v>2634</v>
+        <v>2633</v>
       </c>
       <c r="E390" s="46" t="s">
         <v>2228</v>
@@ -18771,7 +18771,7 @@
         <v>1507</v>
       </c>
       <c r="D396" s="46" t="s">
-        <v>2635</v>
+        <v>2634</v>
       </c>
       <c r="E396" s="46" t="s">
         <v>2019</v>
@@ -18876,7 +18876,7 @@
         <v>1510</v>
       </c>
       <c r="D401" s="46" t="s">
-        <v>2636</v>
+        <v>2635</v>
       </c>
       <c r="E401" s="46" t="s">
         <v>2020</v>
@@ -19548,7 +19548,7 @@
         <v>1526</v>
       </c>
       <c r="D433" s="46" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
       <c r="E433" s="46" t="s">
         <v>2318</v>
@@ -34782,8 +34782,8 @@
   </sheetPr>
   <dimension ref="A1:AB48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="F14" zoomScale="59" zoomScaleNormal="37" zoomScaleSheetLayoutView="73" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="D28" zoomScale="56" zoomScaleNormal="37" zoomScaleSheetLayoutView="73" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -34941,7 +34941,7 @@
         <v>110</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>2598</v>
+        <v>2597</v>
       </c>
       <c r="L6" s="23" t="s">
         <v>111</v>
@@ -34965,7 +34965,7 @@
         <v>117</v>
       </c>
       <c r="S6" s="69" t="s">
-        <v>2614</v>
+        <v>2613</v>
       </c>
     </row>
     <row r="7" spans="1:28" s="22" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -35919,7 +35919,7 @@
         <v>Concluída</v>
       </c>
       <c r="R21" s="44" t="s">
-        <v>2596</v>
+        <v>2637</v>
       </c>
       <c r="S21" s="70">
         <v>45357</v>
@@ -35936,7 +35936,7 @@
         <v>362</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>2601</v>
+        <v>2600</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>2205</v>
@@ -35997,7 +35997,7 @@
         <v>368</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>2602</v>
+        <v>2601</v>
       </c>
       <c r="E23" s="17" t="s">
         <v>2205</v>
@@ -36339,10 +36339,10 @@
       <c r="P28" s="60"/>
       <c r="Q28" s="21" t="str">
         <f ca="1">IF(Prontidao_MedioPrazo[[#This Row],[RESTRIÇÃO DETECTADA]]&lt;&gt;"",IF(Prontidao_MedioPrazo[[#This Row],[TÉRMINO REAL]]&lt;&gt;0,"Concluída",IF(Prontidao_MedioPrazo[[#This Row],[TÉRMINO PREVISTO]]="","À definir",IF(Prontidao_MedioPrazo[[#This Row],[TÉRMINO PREVISTO]]&gt;=TODAY(),"No Prazo","Atrasada"))),"")</f>
-        <v>No Prazo</v>
+        <v>Atrasada</v>
       </c>
       <c r="R28" s="65" t="s">
-        <v>2597</v>
+        <v>2596</v>
       </c>
       <c r="S28" s="70">
         <v>45351</v>
@@ -36359,7 +36359,7 @@
         <v>331</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>2603</v>
+        <v>2602</v>
       </c>
       <c r="E29" s="17" t="s">
         <v>124</v>
@@ -36397,10 +36397,12 @@
         <f>IF(Prontidao_MedioPrazo[[#This Row],[TÉRMINO PREV. (BASELINE)]]="","",Prontidao_MedioPrazo[[#This Row],[TÉRMINO PREV. (BASELINE)]])</f>
         <v>45337</v>
       </c>
-      <c r="P29" s="60"/>
+      <c r="P29" s="60">
+        <v>45345</v>
+      </c>
       <c r="Q29" s="21" t="str">
         <f ca="1">IF(Prontidao_MedioPrazo[[#This Row],[RESTRIÇÃO DETECTADA]]&lt;&gt;"",IF(Prontidao_MedioPrazo[[#This Row],[TÉRMINO REAL]]&lt;&gt;0,"Concluída",IF(Prontidao_MedioPrazo[[#This Row],[TÉRMINO PREVISTO]]="","À definir",IF(Prontidao_MedioPrazo[[#This Row],[TÉRMINO PREVISTO]]&gt;=TODAY(),"No Prazo","Atrasada"))),"")</f>
-        <v>Atrasada</v>
+        <v>Concluída</v>
       </c>
       <c r="R29" s="65" t="s">
         <v>2586</v>
@@ -36420,7 +36422,7 @@
         <v>345</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="E30" s="17" t="s">
         <v>124</v>
@@ -36458,10 +36460,12 @@
         <f>IF(Prontidao_MedioPrazo[[#This Row],[TÉRMINO PREV. (BASELINE)]]="","",Prontidao_MedioPrazo[[#This Row],[TÉRMINO PREV. (BASELINE)]])</f>
         <v>45337</v>
       </c>
-      <c r="P30" s="60"/>
+      <c r="P30" s="60">
+        <v>45345</v>
+      </c>
       <c r="Q30" s="21" t="str">
         <f ca="1">IF(Prontidao_MedioPrazo[[#This Row],[RESTRIÇÃO DETECTADA]]&lt;&gt;"",IF(Prontidao_MedioPrazo[[#This Row],[TÉRMINO REAL]]&lt;&gt;0,"Concluída",IF(Prontidao_MedioPrazo[[#This Row],[TÉRMINO PREVISTO]]="","À definir",IF(Prontidao_MedioPrazo[[#This Row],[TÉRMINO PREVISTO]]&gt;=TODAY(),"No Prazo","Atrasada"))),"")</f>
-        <v>Atrasada</v>
+        <v>Concluída</v>
       </c>
       <c r="R30" s="65" t="s">
         <v>2586</v>
@@ -36488,10 +36492,10 @@
         <v>124</v>
       </c>
       <c r="F31" s="17" t="s">
+        <v>2598</v>
+      </c>
+      <c r="G31" s="18" t="s">
         <v>2599</v>
-      </c>
-      <c r="G31" s="18" t="s">
-        <v>2600</v>
       </c>
       <c r="H31" s="19">
         <v>45342</v>
@@ -36548,10 +36552,10 @@
         <v>124</v>
       </c>
       <c r="F32" s="17" t="s">
+        <v>2598</v>
+      </c>
+      <c r="G32" s="18" t="s">
         <v>2599</v>
-      </c>
-      <c r="G32" s="18" t="s">
-        <v>2600</v>
       </c>
       <c r="H32" s="19">
         <v>45342</v>
@@ -36595,7 +36599,7 @@
         <v>27</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>2608</v>
+        <v>2607</v>
       </c>
       <c r="C33" s="67" t="s">
         <v>54</v>
@@ -36608,10 +36612,10 @@
         <v>124</v>
       </c>
       <c r="F33" s="17" t="s">
+        <v>2598</v>
+      </c>
+      <c r="G33" s="18" t="s">
         <v>2599</v>
-      </c>
-      <c r="G33" s="18" t="s">
-        <v>2600</v>
       </c>
       <c r="H33" s="19">
         <v>45342</v>
@@ -36647,7 +36651,7 @@
         <v>28</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>2608</v>
+        <v>2607</v>
       </c>
       <c r="C34" s="67" t="s">
         <v>280</v>
@@ -36660,10 +36664,10 @@
         <v>124</v>
       </c>
       <c r="F34" s="17" t="s">
+        <v>2598</v>
+      </c>
+      <c r="G34" s="18" t="s">
         <v>2599</v>
-      </c>
-      <c r="G34" s="18" t="s">
-        <v>2600</v>
       </c>
       <c r="H34" s="19">
         <v>45342</v>
@@ -36699,7 +36703,7 @@
         <v>29</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>2608</v>
+        <v>2607</v>
       </c>
       <c r="C35" s="67" t="s">
         <v>281</v>
@@ -36712,10 +36716,10 @@
         <v>124</v>
       </c>
       <c r="F35" s="17" t="s">
+        <v>2598</v>
+      </c>
+      <c r="G35" s="18" t="s">
         <v>2599</v>
-      </c>
-      <c r="G35" s="18" t="s">
-        <v>2600</v>
       </c>
       <c r="H35" s="19">
         <v>45342</v>
@@ -36751,7 +36755,7 @@
         <v>30</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>2608</v>
+        <v>2607</v>
       </c>
       <c r="C36" s="67" t="s">
         <v>174</v>
@@ -36764,10 +36768,10 @@
         <v>124</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>2599</v>
+        <v>2598</v>
       </c>
       <c r="G36" s="18" t="s">
-        <v>2605</v>
+        <v>2604</v>
       </c>
       <c r="H36" s="19">
         <v>45342</v>
@@ -36816,10 +36820,10 @@
         <v>124</v>
       </c>
       <c r="F37" s="17" t="s">
+        <v>2598</v>
+      </c>
+      <c r="G37" s="18" t="s">
         <v>2599</v>
-      </c>
-      <c r="G37" s="18" t="s">
-        <v>2600</v>
       </c>
       <c r="H37" s="19">
         <v>45342</v>
@@ -36833,9 +36837,15 @@
         <f>WEEKNUM(Prontidao_MedioPrazo[[#This Row],[Coluna1]])</f>
         <v>9</v>
       </c>
-      <c r="L37" s="61"/>
-      <c r="M37" s="61"/>
-      <c r="N37" s="62"/>
+      <c r="L37" s="61" t="s">
+        <v>2218</v>
+      </c>
+      <c r="M37" s="61" t="s">
+        <v>2194</v>
+      </c>
+      <c r="N37" s="62" t="s">
+        <v>2193</v>
+      </c>
       <c r="O37" s="63" t="str">
         <f>IF(Prontidao_MedioPrazo[[#This Row],[TÉRMINO PREV. (BASELINE)]]="","",Prontidao_MedioPrazo[[#This Row],[TÉRMINO PREV. (BASELINE)]])</f>
         <v/>
@@ -36868,10 +36878,10 @@
         <v>124</v>
       </c>
       <c r="F38" s="17" t="s">
+        <v>2598</v>
+      </c>
+      <c r="G38" s="18" t="s">
         <v>2599</v>
-      </c>
-      <c r="G38" s="18" t="s">
-        <v>2600</v>
       </c>
       <c r="H38" s="19">
         <v>45342</v>
@@ -36885,9 +36895,15 @@
         <f>WEEKNUM(Prontidao_MedioPrazo[[#This Row],[Coluna1]])</f>
         <v>10</v>
       </c>
-      <c r="L38" s="61"/>
-      <c r="M38" s="61"/>
-      <c r="N38" s="62"/>
+      <c r="L38" s="61" t="s">
+        <v>2218</v>
+      </c>
+      <c r="M38" s="61" t="s">
+        <v>2194</v>
+      </c>
+      <c r="N38" s="62" t="s">
+        <v>2193</v>
+      </c>
       <c r="O38" s="63" t="str">
         <f>IF(Prontidao_MedioPrazo[[#This Row],[TÉRMINO PREV. (BASELINE)]]="","",Prontidao_MedioPrazo[[#This Row],[TÉRMINO PREV. (BASELINE)]])</f>
         <v/>
@@ -36913,13 +36929,13 @@
         <v>374</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>2606</v>
+        <v>2605</v>
       </c>
       <c r="E39" s="17" t="s">
         <v>124</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>2609</v>
+        <v>2608</v>
       </c>
       <c r="G39" s="18" t="s">
         <v>2206</v>
@@ -36966,7 +36982,7 @@
         <v>399</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>2607</v>
+        <v>2606</v>
       </c>
       <c r="E40" s="17" t="s">
         <v>2205</v>
@@ -37013,7 +37029,7 @@
         <v>35</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>2608</v>
+        <v>2607</v>
       </c>
       <c r="C41" s="67" t="s">
         <v>709</v>
@@ -37026,10 +37042,10 @@
         <v>124</v>
       </c>
       <c r="F41" s="17" t="s">
+        <v>2598</v>
+      </c>
+      <c r="G41" s="18" t="s">
         <v>2599</v>
-      </c>
-      <c r="G41" s="18" t="s">
-        <v>2600</v>
       </c>
       <c r="H41" s="19">
         <v>45342</v>
@@ -37065,7 +37081,7 @@
         <v>36</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>2608</v>
+        <v>2607</v>
       </c>
       <c r="C42" s="67" t="s">
         <v>718</v>
@@ -37078,10 +37094,10 @@
         <v>124</v>
       </c>
       <c r="F42" s="17" t="s">
+        <v>2598</v>
+      </c>
+      <c r="G42" s="18" t="s">
         <v>2599</v>
-      </c>
-      <c r="G42" s="18" t="s">
-        <v>2600</v>
       </c>
       <c r="H42" s="19">
         <v>45342</v>
@@ -37117,7 +37133,7 @@
         <v>37</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>2608</v>
+        <v>2607</v>
       </c>
       <c r="C43" s="67" t="s">
         <v>726</v>
@@ -37130,10 +37146,10 @@
         <v>124</v>
       </c>
       <c r="F43" s="17" t="s">
+        <v>2598</v>
+      </c>
+      <c r="G43" s="18" t="s">
         <v>2599</v>
-      </c>
-      <c r="G43" s="18" t="s">
-        <v>2600</v>
       </c>
       <c r="H43" s="19">
         <v>45342</v>
@@ -37169,7 +37185,7 @@
         <v>38</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>2608</v>
+        <v>2607</v>
       </c>
       <c r="C44" s="67" t="s">
         <v>754</v>
@@ -37182,10 +37198,10 @@
         <v>124</v>
       </c>
       <c r="F44" s="17" t="s">
+        <v>2598</v>
+      </c>
+      <c r="G44" s="18" t="s">
         <v>2599</v>
-      </c>
-      <c r="G44" s="18" t="s">
-        <v>2600</v>
       </c>
       <c r="H44" s="19">
         <v>45342</v>
@@ -37234,10 +37250,10 @@
         <v>124</v>
       </c>
       <c r="F45" s="17" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
       <c r="G45" s="18" t="s">
-        <v>2612</v>
+        <v>2611</v>
       </c>
       <c r="H45" s="19">
         <v>45342</v>
@@ -37286,10 +37302,10 @@
         <v>124</v>
       </c>
       <c r="F46" s="17" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
       <c r="G46" s="18" t="s">
-        <v>2612</v>
+        <v>2611</v>
       </c>
       <c r="H46" s="19">
         <v>45342</v>
@@ -37303,9 +37319,15 @@
         <f>WEEKNUM(Prontidao_MedioPrazo[[#This Row],[Coluna1]])</f>
         <v>9</v>
       </c>
-      <c r="L46" s="61"/>
-      <c r="M46" s="61"/>
-      <c r="N46" s="62"/>
+      <c r="L46" s="61" t="s">
+        <v>2218</v>
+      </c>
+      <c r="M46" s="61" t="s">
+        <v>2194</v>
+      </c>
+      <c r="N46" s="62" t="s">
+        <v>2193</v>
+      </c>
       <c r="O46" s="63" t="str">
         <f>IF(Prontidao_MedioPrazo[[#This Row],[TÉRMINO PREV. (BASELINE)]]="","",Prontidao_MedioPrazo[[#This Row],[TÉRMINO PREV. (BASELINE)]])</f>
         <v/>
@@ -37331,16 +37353,16 @@
         <v>1095</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>2610</v>
+        <v>2609</v>
       </c>
       <c r="E47" s="17" t="s">
         <v>124</v>
       </c>
       <c r="F47" s="17" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
       <c r="G47" s="18" t="s">
-        <v>2612</v>
+        <v>2611</v>
       </c>
       <c r="H47" s="19">
         <v>45342</v>
@@ -37354,9 +37376,15 @@
         <f>WEEKNUM(Prontidao_MedioPrazo[[#This Row],[Coluna1]])</f>
         <v>10</v>
       </c>
-      <c r="L47" s="61"/>
-      <c r="M47" s="61"/>
-      <c r="N47" s="62"/>
+      <c r="L47" s="61" t="s">
+        <v>2218</v>
+      </c>
+      <c r="M47" s="61" t="s">
+        <v>2194</v>
+      </c>
+      <c r="N47" s="62" t="s">
+        <v>2193</v>
+      </c>
       <c r="O47" s="63" t="str">
         <f>IF(Prontidao_MedioPrazo[[#This Row],[TÉRMINO PREV. (BASELINE)]]="","",Prontidao_MedioPrazo[[#This Row],[TÉRMINO PREV. (BASELINE)]])</f>
         <v/>
@@ -37382,16 +37410,16 @@
         <v>1101</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>2611</v>
+        <v>2610</v>
       </c>
       <c r="E48" s="17" t="s">
         <v>124</v>
       </c>
       <c r="F48" s="17" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
       <c r="G48" s="18" t="s">
-        <v>2612</v>
+        <v>2611</v>
       </c>
       <c r="H48" s="19">
         <v>45342</v>
@@ -37405,9 +37433,15 @@
         <f>WEEKNUM(Prontidao_MedioPrazo[[#This Row],[Coluna1]])</f>
         <v>11</v>
       </c>
-      <c r="L48" s="61"/>
-      <c r="M48" s="61"/>
-      <c r="N48" s="62"/>
+      <c r="L48" s="61" t="s">
+        <v>2218</v>
+      </c>
+      <c r="M48" s="61" t="s">
+        <v>2194</v>
+      </c>
+      <c r="N48" s="62" t="s">
+        <v>2193</v>
+      </c>
       <c r="O48" s="63" t="str">
         <f>IF(Prontidao_MedioPrazo[[#This Row],[TÉRMINO PREV. (BASELINE)]]="","",Prontidao_MedioPrazo[[#This Row],[TÉRMINO PREV. (BASELINE)]])</f>
         <v/>
@@ -38008,6 +38042,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="601ddd3e-e7e7-4b57-95a9-114b343b906a" xsi:nil="true"/>
@@ -38017,15 +38060,6 @@
     <DocumentCategory xmlns="e7640078-2807-4792-8712-763d4cb58983" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -38253,6 +38287,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F1CA883-11A7-4649-9521-EA04A9666402}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED4F5EE1-56D7-4FFB-B992-DE488B5495B9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -38260,14 +38302,6 @@
     <ds:schemaRef ds:uri="601ddd3e-e7e7-4b57-95a9-114b343b906a"/>
     <ds:schemaRef ds:uri="acfac000-05a5-4485-98d1-25ae80f2ac3c"/>
     <ds:schemaRef ds:uri="e7640078-2807-4792-8712-763d4cb58983"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F1CA883-11A7-4649-9521-EA04A9666402}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>